<commit_message>
added data from one project into the table, title points to current location on wisc
</commit_message>
<xml_diff>
--- a/2.0/data/datatable.xlsx
+++ b/2.0/data/datatable.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="2325"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="370 Projects" sheetId="1" r:id="rId1"/>
+    <sheet name="Research" sheetId="2" r:id="rId2"/>
+    <sheet name="572 Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="575 Projects" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="153">
   <si>
     <t>Title</t>
   </si>
@@ -54,18 +57,6 @@
   </si>
   <si>
     <t>Keyword3</t>
-  </si>
-  <si>
-    <t>Keyword4</t>
-  </si>
-  <si>
-    <t>Keyword5</t>
-  </si>
-  <si>
-    <t>Keyword6</t>
-  </si>
-  <si>
-    <t>Keyword7</t>
   </si>
   <si>
     <t>Source (URL or file location?)</t>
@@ -309,6 +300,213 @@
   </si>
   <si>
     <t>Allison Grumley</t>
+  </si>
+  <si>
+    <t>Travis Wickboldt</t>
+  </si>
+  <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Trans-Alaska Pipeline System</t>
+  </si>
+  <si>
+    <t>Tyler Peterka</t>
+  </si>
+  <si>
+    <t>The York Factory Express</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>Individual Mobility and Political Activism</t>
+  </si>
+  <si>
+    <t>Peter Swift</t>
+  </si>
+  <si>
+    <t>Tom Cox</t>
+  </si>
+  <si>
+    <t>Sasquatch Sightings in the US</t>
+  </si>
+  <si>
+    <t>dot</t>
+  </si>
+  <si>
+    <t>The Blue Mounds</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Tim Rooney</t>
+  </si>
+  <si>
+    <t>Give and Take: Shifts in Federal Deficit Spending, 1981-2005</t>
+  </si>
+  <si>
+    <t>Steve Paling</t>
+  </si>
+  <si>
+    <t>Randy Benetzke</t>
+  </si>
+  <si>
+    <t>NO TITLE: Eastern Independence to the West Coast the United States 70 Years of Land Acquisition, State Boundaries as Established over 125 Years, Timeline of When A Territory Enter the Union of the United States as a State</t>
+  </si>
+  <si>
+    <t>timeline</t>
+  </si>
+  <si>
+    <t>Bringing Organic Produce to Market</t>
+  </si>
+  <si>
+    <t>Rachel Boothby</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>health</t>
+  </si>
+  <si>
+    <t>United Migrant Opportunity Services: Building Better Futures</t>
+  </si>
+  <si>
+    <t>Peter Bauknecht</t>
+  </si>
+  <si>
+    <t>nonprofit</t>
+  </si>
+  <si>
+    <t>blurb(containing keywords?)</t>
+  </si>
+  <si>
+    <t>Study Abroad International Academic Programs University of Wisconsin-Madison</t>
+  </si>
+  <si>
+    <t>Molly Trerotola</t>
+  </si>
+  <si>
+    <t>travel</t>
+  </si>
+  <si>
+    <t>Revenue from Endangered Species Protection within state National Parks, 2011</t>
+  </si>
+  <si>
+    <t>proportional symbol, choropleth</t>
+  </si>
+  <si>
+    <t>Molly Ryan</t>
+  </si>
+  <si>
+    <t>Still a Melting Pot: Immigration to the US, 2010</t>
+  </si>
+  <si>
+    <t>Mikaela Weiss</t>
+  </si>
+  <si>
+    <t>Luke Albers</t>
+  </si>
+  <si>
+    <t>US Drone Strikes in Yemen</t>
+  </si>
+  <si>
+    <t>How Much is Enough?</t>
+  </si>
+  <si>
+    <t>cartogram, choropleth</t>
+  </si>
+  <si>
+    <t>MakieMatsumoto Hervol</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>Katie Ginther</t>
+  </si>
+  <si>
+    <t>Impacts and Near-Misses: Asteroids, Meteoroids and Their Impact Craters on Planet Earth</t>
+  </si>
+  <si>
+    <t>dot, proportional symbol</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>50 Years of Badgers: Freshman Enrollment 1962 and 2012</t>
+  </si>
+  <si>
+    <t>Lowell Fissinger</t>
+  </si>
+  <si>
+    <t>split symbol, proportional symbol</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>Ski North America</t>
+  </si>
+  <si>
+    <t>isoline</t>
+  </si>
+  <si>
+    <t>Lindsay Frensz</t>
+  </si>
+  <si>
+    <t>weather</t>
+  </si>
+  <si>
+    <t>Eric Jeng</t>
+  </si>
+  <si>
+    <t>Rebalancing in Asia: US Military in the West Pacific</t>
+  </si>
+  <si>
+    <t>reference, proportional symbol</t>
+  </si>
+  <si>
+    <t>Joey Snarski</t>
+  </si>
+  <si>
+    <t>Investigating Dixie Alley: Tornado tracks from 1950 through 2011</t>
+  </si>
+  <si>
+    <t>goMilwaukee</t>
+  </si>
+  <si>
+    <t>bivariate choropleth</t>
+  </si>
+  <si>
+    <t>Joe Minik</t>
+  </si>
+  <si>
+    <t>rent</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>Jessie Conaway</t>
+  </si>
+  <si>
+    <t>Protect Our Water, Protect Ourselves: Ecosystem Threats and Breast Cancer Rates in Wisconsin Watersheds</t>
+  </si>
+  <si>
+    <t>James Rollo</t>
+  </si>
+  <si>
+    <t>The Global Premier League: A Comparison of English Premier League Players' Birthplaces with National Affluence</t>
+  </si>
+  <si>
+    <t>Emily Pauly</t>
+  </si>
+  <si>
+    <t>Money Can't Buy You Votes</t>
   </si>
 </sst>
 </file>
@@ -632,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -645,15 +843,15 @@
     <col min="4" max="4" width="15.73046875" customWidth="1"/>
     <col min="5" max="5" width="13.9296875" customWidth="1"/>
     <col min="6" max="6" width="13.19921875" customWidth="1"/>
-    <col min="16" max="16" width="24.265625" customWidth="1"/>
+    <col min="13" max="13" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -683,767 +881,1428 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2">
+        <v>2012</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2">
-        <v>2012</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>2012</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4">
+        <v>2012</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3">
-        <v>2012</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
+        <v>2012</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>2012</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6">
+        <v>2012</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5">
-        <v>2012</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7">
+        <v>2012</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>2012</v>
-      </c>
-      <c r="G6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>2012</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7">
-        <v>2012</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>2012</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8">
-        <v>2012</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>2012</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9">
-        <v>2012</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>2012</v>
+      </c>
+      <c r="G11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>2012</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>2012</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
         <v>41</v>
       </c>
-      <c r="J9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10">
-        <v>2012</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>2012</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15">
+        <v>2012</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11">
-        <v>2012</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12">
-        <v>2012</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13">
-        <v>2012</v>
-      </c>
-      <c r="G13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>41</v>
-      </c>
-      <c r="J13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14">
-        <v>2012</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>2012</v>
+      </c>
+      <c r="G16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15">
-        <v>2012</v>
-      </c>
-      <c r="G15" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16">
-        <v>2012</v>
-      </c>
-      <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F17">
         <v>2012</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F18">
         <v>2012</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F19">
         <v>2012</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F20">
         <v>2012</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F21">
         <v>2012</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F22">
         <v>2012</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F23">
         <v>2012</v>
       </c>
       <c r="G23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F24">
         <v>2012</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F25">
         <v>2012</v>
       </c>
       <c r="G25" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F26">
         <v>2012</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F27">
         <v>2012</v>
       </c>
       <c r="G27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F28">
         <v>2012</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F29">
         <v>2012</v>
       </c>
       <c r="G29" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="I29" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F30">
         <v>2012</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31">
+        <v>2012</v>
+      </c>
+      <c r="G31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
         <v>84</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32">
+        <v>2012</v>
+      </c>
+      <c r="G32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
         <v>87</v>
       </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="F31">
-        <v>2012</v>
-      </c>
-      <c r="G31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" t="s">
-        <v>19</v>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33">
+        <v>2012</v>
+      </c>
+      <c r="G33" t="s">
+        <v>85</v>
+      </c>
+      <c r="H33" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34">
+        <v>2012</v>
+      </c>
+      <c r="G34" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35">
+        <v>2012</v>
+      </c>
+      <c r="G35" t="s">
+        <v>85</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="B36" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36">
+        <v>2012</v>
+      </c>
+      <c r="G36" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37">
+        <v>2012</v>
+      </c>
+      <c r="G37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38">
+        <v>2012</v>
+      </c>
+      <c r="G38" t="s">
+        <v>85</v>
+      </c>
+      <c r="H38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39">
+        <v>2012</v>
+      </c>
+      <c r="G39" t="s">
+        <v>85</v>
+      </c>
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>105</v>
+      </c>
+      <c r="J39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40">
+        <v>2012</v>
+      </c>
+      <c r="G40" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41">
+        <v>2012</v>
+      </c>
+      <c r="G41" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42">
+        <v>2012</v>
+      </c>
+      <c r="G42" t="s">
+        <v>85</v>
+      </c>
+      <c r="H42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43">
+        <v>2012</v>
+      </c>
+      <c r="G43" t="s">
+        <v>85</v>
+      </c>
+      <c r="H43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44">
+        <v>2012</v>
+      </c>
+      <c r="G44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45">
+        <v>2012</v>
+      </c>
+      <c r="G45" t="s">
+        <v>85</v>
+      </c>
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46">
+        <v>2012</v>
+      </c>
+      <c r="G46" t="s">
+        <v>85</v>
+      </c>
+      <c r="H46" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>129</v>
+      </c>
+      <c r="B47" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47">
+        <v>2012</v>
+      </c>
+      <c r="G47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48">
+        <v>2012</v>
+      </c>
+      <c r="G48" t="s">
+        <v>85</v>
+      </c>
+      <c r="H48" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49">
+        <v>2012</v>
+      </c>
+      <c r="G49" t="s">
+        <v>85</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <v>2012</v>
+      </c>
+      <c r="G50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H50" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>142</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="C51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51">
+        <v>2012</v>
+      </c>
+      <c r="G51" t="s">
+        <v>85</v>
+      </c>
+      <c r="H51" t="s">
+        <v>15</v>
+      </c>
+      <c r="I51" t="s">
+        <v>145</v>
+      </c>
+      <c r="J51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52">
+        <v>2012</v>
+      </c>
+      <c r="G52" t="s">
+        <v>85</v>
+      </c>
+      <c r="H52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53">
+        <v>2012</v>
+      </c>
+      <c r="G53" t="s">
+        <v>85</v>
+      </c>
+      <c r="H53" t="s">
+        <v>15</v>
+      </c>
+      <c r="I53" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54">
+        <v>2012</v>
+      </c>
+      <c r="G54" t="s">
+        <v>85</v>
+      </c>
+      <c r="H54" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M50">
+    <sortCondition sortBy="icon" ref="A51"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data entry, added ugliest search box of all time, unsuccessfuly tried to fix datatable
</commit_message>
<xml_diff>
--- a/2.0/data/datatable.xlsx
+++ b/2.0/data/datatable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="2325"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="2325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="370 Projects" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="226">
   <si>
     <t>Title</t>
   </si>
@@ -39,9 +39,6 @@
   </si>
   <si>
     <t>Semester</t>
-  </si>
-  <si>
-    <t>Source (URL or file location?)</t>
   </si>
   <si>
     <t>Treading Water: The Dutch Reliance on Water Management</t>
@@ -522,6 +519,213 @@
   </si>
   <si>
     <t>Jessica Shen</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Edinburgh Marathon Course Map</t>
+  </si>
+  <si>
+    <t>Jacqueline Heller</t>
+  </si>
+  <si>
+    <t>sports, elevation, race</t>
+  </si>
+  <si>
+    <t>The Alphorn-Man Triathlon of New Glarus</t>
+  </si>
+  <si>
+    <t>Jackson Gabriel</t>
+  </si>
+  <si>
+    <t>sports, race</t>
+  </si>
+  <si>
+    <t>Greg Lehner</t>
+  </si>
+  <si>
+    <t>How Many Big Macs Can You Buy?</t>
+  </si>
+  <si>
+    <t>economics, world map, gross domestic product</t>
+  </si>
+  <si>
+    <t>Mammal Diversity of North America</t>
+  </si>
+  <si>
+    <t>Grace Shellinger</t>
+  </si>
+  <si>
+    <t>The Frontline of the Battle Against Asian Carp in the Great Lakes Drainage Basin</t>
+  </si>
+  <si>
+    <t>Erin Hamilton</t>
+  </si>
+  <si>
+    <t>environment, invasive species</t>
+  </si>
+  <si>
+    <t>David Rhoten</t>
+  </si>
+  <si>
+    <t>Reconstructing Iraq, Summer 2003: 928 Engineer Group Survey and Design</t>
+  </si>
+  <si>
+    <t>Syria, Turkey, Iraq, Middle East</t>
+  </si>
+  <si>
+    <t>October 2011 Northern Hemisphere Jets and Superpositions</t>
+  </si>
+  <si>
+    <t>Croix Christenson</t>
+  </si>
+  <si>
+    <t>weather, meteorology, polar jet, subtropical jet, choropleth</t>
+  </si>
+  <si>
+    <t>Protecting the Penokee Range from Irresponsible Iron Mining</t>
+  </si>
+  <si>
+    <t>Christy Stamos</t>
+  </si>
+  <si>
+    <t>Wisconsin, Madison, Green Bay, Milwaukee, Wisconsin League of Conservation Voters</t>
+  </si>
+  <si>
+    <t>Casey Dahl</t>
+  </si>
+  <si>
+    <t>What Is Local? Dane County Farmers Market Vendor Locations in 2009</t>
+  </si>
+  <si>
+    <t>farmer's market, local food, health, Dane County Farmers' Market, choropleth</t>
+  </si>
+  <si>
+    <t>Blake Draper</t>
+  </si>
+  <si>
+    <t>Mapping a Watershed: Three Views of the Yahara Watershed for Public Outreach and Education</t>
+  </si>
+  <si>
+    <t>choropleth, dot density</t>
+  </si>
+  <si>
+    <t>America's Pastime? Wins, Ticket Price, and Attendance for Major League Baseball Franchises, 2011</t>
+  </si>
+  <si>
+    <t>Bryan Plaster</t>
+  </si>
+  <si>
+    <t>proportional symbol, choropleth, United States, spors</t>
+  </si>
+  <si>
+    <t>The Dirty Truth About Coal</t>
+  </si>
+  <si>
+    <t>Amanda Kannard</t>
+  </si>
+  <si>
+    <t>coal plants, Wisconsin, proportional symbol, bivariate choropleth, health, respiratory disease</t>
+  </si>
+  <si>
+    <t>Spain's Influence on the World</t>
+  </si>
+  <si>
+    <t>Ari Malman</t>
+  </si>
+  <si>
+    <t>language, world map, choropleth, history</t>
+  </si>
+  <si>
+    <t>Research</t>
+  </si>
+  <si>
+    <t>Robinson AC and RE Roth</t>
+  </si>
+  <si>
+    <t>Buckingham TMA and RE Roth.</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Special Issue on Cognition, Representation, and Behavior sponsored by the International Cartography Association (ICA).</t>
+  </si>
+  <si>
+    <t>Second Special Digital Issue.</t>
+  </si>
+  <si>
+    <t>Cartographic Perspectives 66. [open access]</t>
+  </si>
+  <si>
+    <t>Cartographic Perspectives 77. [open access]</t>
+  </si>
+  <si>
+    <t>Wireframing for interactive &amp; web-based mapping: Designing the NOAA Lake Level Viewer. </t>
+  </si>
+  <si>
+    <t>Cartography and Geographic Information Science</t>
+  </si>
+  <si>
+    <t>Roth RE. </t>
+  </si>
+  <si>
+    <t>Roth RE, D Hart, R Mead, and C Quinn.</t>
+  </si>
+  <si>
+    <t>forthcoming</t>
+  </si>
+  <si>
+    <t>Cartographica. 50(2).</t>
+  </si>
+  <si>
+    <t>Interactivity and Cartography: A contemporary perspective on UI/UX design from geospatial professionals. </t>
+  </si>
+  <si>
+    <t>Tambopata transformed: Using web mapping to enhance a geography course exercise about forest conservation. </t>
+  </si>
+  <si>
+    <t>Weiss MJ, M Omri, G White, RE Roth, and LC Naughton-Treves. 2015.</t>
+  </si>
+  <si>
+    <t>The Journal of Maps. 11(3): 525-533. [uncorrected pre-print]</t>
+  </si>
+  <si>
+    <t>User-centered design for interactive maps: A case study in crime analysis. </t>
+  </si>
+  <si>
+    <t>Roth RE, KS Ross, and AM MacEachren.</t>
+  </si>
+  <si>
+    <t> International Journal of Geo-Information. 4(1): 262-301. [open access]</t>
+  </si>
+  <si>
+    <t>Roth RE, C Quinn, and D Hart. 2015.</t>
+  </si>
+  <si>
+    <t>The competitive analysis method for evaluating water level visualization tools.</t>
+  </si>
+  <si>
+    <t>In: A. Vondrakova, J. Brus, and V. Vozenilek (eds) Modern Trends in Cartography, Lecture Notes in Geoinformation and Cartography. Chapter 19: 241-256. [uncorrected pre-print]</t>
+  </si>
+  <si>
+    <t>Roth RE, RG Donohue, CM Sack, T Wallace, and T Buckingham.</t>
+  </si>
+  <si>
+    <t>Keeping pace with evolving open source web mapping technologies.</t>
+  </si>
+  <si>
+    <t>Dong W, H Liao, RE Roth, and S Wang.</t>
+  </si>
+  <si>
+    <t>Cartographic Perspectives. 78: 25-52. [open access]</t>
+  </si>
+  <si>
+    <t>Eye tracking to explore the potential of enhanced imagery basemaps in web mapping.</t>
+  </si>
+  <si>
+    <t>The Cartographic Journal. 51(4): 313-329. [uncorrected pre-print]</t>
   </si>
 </sst>
 </file>
@@ -658,6 +862,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -693,6 +914,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -845,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -859,12 +1097,12 @@
     <col min="10" max="10" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -876,1377 +1114,1634 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
-      </c>
-      <c r="J1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>2012</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>2012</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="C3">
+        <v>2012</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>2012</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>2012</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
-        <v>2012</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>2012</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
-        <v>2012</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>2012</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
-        <v>2012</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="C7">
+        <v>2012</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>2012</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="C8">
+        <v>2012</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>2012</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>2012</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
-        <v>2012</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="C10">
+        <v>2012</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10">
-        <v>2012</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="C11">
+        <v>2012</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11">
-        <v>2012</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12">
+        <v>2012</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
         <v>28</v>
       </c>
-      <c r="C12">
-        <v>2012</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="C13">
+        <v>2012</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>2012</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14">
+        <v>2012</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>32</v>
       </c>
-      <c r="C14">
-        <v>2012</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15">
+        <v>2012</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C15">
-        <v>2012</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
       <c r="C16">
         <v>2012</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
       <c r="C17">
         <v>2012</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>2012</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>2012</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
       <c r="C20">
         <v>2012</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>46</v>
-      </c>
       <c r="C21">
         <v>2012</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
       <c r="C22">
         <v>2012</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24">
         <v>2012</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25">
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="B26" t="s">
-        <v>56</v>
-      </c>
       <c r="C26">
         <v>2012</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
       <c r="C27">
         <v>2012</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
       <c r="C28">
         <v>2012</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29">
         <v>2012</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
         <v>63</v>
       </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
       <c r="C30">
         <v>2012</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
-        <v>66</v>
-      </c>
       <c r="C31">
         <v>2012</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C32">
         <v>2012</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33">
         <v>2012</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="B34" t="s">
-        <v>73</v>
-      </c>
       <c r="C34">
         <v>2012</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C35">
         <v>2012</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="B36" t="s">
-        <v>77</v>
-      </c>
       <c r="C36">
         <v>2012</v>
       </c>
       <c r="D36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
         <v>78</v>
       </c>
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
       <c r="C37">
         <v>2012</v>
       </c>
       <c r="D37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38">
         <v>2012</v>
       </c>
       <c r="D38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
         <v>82</v>
       </c>
-      <c r="B39" t="s">
-        <v>83</v>
-      </c>
       <c r="C39">
         <v>2012</v>
       </c>
       <c r="D39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
         <v>84</v>
       </c>
-      <c r="B40" t="s">
-        <v>85</v>
-      </c>
       <c r="C40">
         <v>2012</v>
       </c>
       <c r="D40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
         <v>86</v>
       </c>
-      <c r="B41" t="s">
-        <v>87</v>
-      </c>
       <c r="C41">
         <v>2012</v>
       </c>
       <c r="D41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
         <v>88</v>
       </c>
-      <c r="B42" t="s">
-        <v>89</v>
-      </c>
       <c r="C42">
         <v>2012</v>
       </c>
       <c r="D42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" t="s">
         <v>90</v>
       </c>
-      <c r="B43" t="s">
-        <v>91</v>
-      </c>
       <c r="C43">
         <v>2012</v>
       </c>
       <c r="D43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C44">
         <v>2012</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
         <v>94</v>
       </c>
-      <c r="B45" t="s">
-        <v>95</v>
-      </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
         <v>98</v>
       </c>
-      <c r="B47" t="s">
-        <v>99</v>
-      </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" t="s">
         <v>100</v>
       </c>
-      <c r="B48" t="s">
-        <v>101</v>
-      </c>
       <c r="C48">
         <v>2012</v>
       </c>
       <c r="D48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>2012</v>
       </c>
       <c r="D49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50">
         <v>2012</v>
       </c>
       <c r="D50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51" t="s">
         <v>106</v>
       </c>
-      <c r="B51" t="s">
-        <v>107</v>
-      </c>
       <c r="C51">
         <v>2012</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52">
         <v>2012</v>
       </c>
       <c r="D52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G52" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C53">
         <v>2012</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54">
         <v>2012</v>
       </c>
       <c r="D54" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C55">
         <v>2011</v>
       </c>
       <c r="D55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C56">
         <v>2011</v>
       </c>
       <c r="D56" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
+        <v>122</v>
+      </c>
+      <c r="B57" t="s">
         <v>123</v>
-      </c>
-      <c r="B57" t="s">
-        <v>124</v>
       </c>
       <c r="C57">
         <v>2011</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" t="s">
         <v>126</v>
-      </c>
-      <c r="B58" t="s">
-        <v>127</v>
       </c>
       <c r="C58">
         <v>2011</v>
       </c>
       <c r="D58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C59">
         <v>2011</v>
       </c>
       <c r="D59" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
+        <v>131</v>
+      </c>
+      <c r="B60" t="s">
         <v>132</v>
-      </c>
-      <c r="B60" t="s">
-        <v>133</v>
       </c>
       <c r="C60">
         <v>2011</v>
       </c>
       <c r="D60" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C61">
         <v>2011</v>
       </c>
       <c r="D61" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C62">
         <v>2011</v>
       </c>
       <c r="D62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G62" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" t="s">
         <v>141</v>
-      </c>
-      <c r="B63" t="s">
-        <v>142</v>
       </c>
       <c r="C63">
         <v>2011</v>
       </c>
       <c r="D63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
+        <v>143</v>
+      </c>
+      <c r="B64" t="s">
         <v>144</v>
-      </c>
-      <c r="B64" t="s">
-        <v>145</v>
       </c>
       <c r="C64">
         <v>2011</v>
       </c>
       <c r="D64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
         <v>147</v>
-      </c>
-      <c r="B65" t="s">
-        <v>148</v>
       </c>
       <c r="C65">
         <v>2011</v>
       </c>
       <c r="D65" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E65" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C66">
         <v>2011</v>
       </c>
       <c r="D66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C67">
         <v>2011</v>
       </c>
       <c r="D67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" t="s">
         <v>156</v>
-      </c>
-      <c r="B68" t="s">
-        <v>157</v>
       </c>
       <c r="C68">
         <v>2011</v>
       </c>
       <c r="D68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>158</v>
+      </c>
+      <c r="B69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69">
+        <v>2011</v>
+      </c>
+      <c r="D69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E69" t="s">
+        <v>7</v>
+      </c>
+      <c r="F69" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>161</v>
+      </c>
+      <c r="B70" t="s">
+        <v>162</v>
+      </c>
+      <c r="C70">
+        <v>2011</v>
+      </c>
+      <c r="D70" t="s">
+        <v>67</v>
+      </c>
+      <c r="E70" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>165</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71">
+        <v>2011</v>
+      </c>
+      <c r="D71" t="s">
+        <v>67</v>
+      </c>
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>167</v>
+      </c>
+      <c r="B72" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72">
+        <v>2011</v>
+      </c>
+      <c r="D72" t="s">
+        <v>67</v>
+      </c>
+      <c r="E72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>169</v>
+      </c>
+      <c r="B73" t="s">
+        <v>170</v>
+      </c>
+      <c r="C73">
+        <v>2011</v>
+      </c>
+      <c r="D73" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" t="s">
+        <v>7</v>
+      </c>
+      <c r="F73" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" t="s">
+        <v>172</v>
+      </c>
+      <c r="C74">
+        <v>2011</v>
+      </c>
+      <c r="D74" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" t="s">
+        <v>176</v>
+      </c>
+      <c r="C75">
+        <v>2011</v>
+      </c>
+      <c r="D75" t="s">
+        <v>67</v>
+      </c>
+      <c r="E75" t="s">
+        <v>7</v>
+      </c>
+      <c r="F75" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" t="s">
+        <v>179</v>
+      </c>
+      <c r="C76">
+        <v>2011</v>
+      </c>
+      <c r="D76" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+      <c r="F76" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>182</v>
+      </c>
+      <c r="B77" t="s">
+        <v>181</v>
+      </c>
+      <c r="C77">
+        <v>2011</v>
+      </c>
+      <c r="D77" t="s">
+        <v>67</v>
+      </c>
+      <c r="E77" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>185</v>
+      </c>
+      <c r="B78" t="s">
+        <v>184</v>
+      </c>
+      <c r="C78">
+        <v>2011</v>
+      </c>
+      <c r="D78" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" t="s">
+        <v>7</v>
+      </c>
+      <c r="F78" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>187</v>
+      </c>
+      <c r="B79" t="s">
+        <v>188</v>
+      </c>
+      <c r="C79">
+        <v>2011</v>
+      </c>
+      <c r="D79" t="s">
+        <v>67</v>
+      </c>
+      <c r="E79" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>190</v>
+      </c>
+      <c r="B80" t="s">
+        <v>191</v>
+      </c>
+      <c r="C80">
+        <v>2011</v>
+      </c>
+      <c r="D80" t="s">
+        <v>67</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>193</v>
+      </c>
+      <c r="B81" t="s">
+        <v>194</v>
+      </c>
+      <c r="C81">
+        <v>2011</v>
+      </c>
+      <c r="D81" t="s">
+        <v>67</v>
+      </c>
+      <c r="E81" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2260,13 +2755,310 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2">
+        <v>2014</v>
+      </c>
+      <c r="D2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G2" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="D3" t="s">
+        <v>199</v>
+      </c>
+      <c r="E3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C4">
+        <v>2014</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+      <c r="E4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6">
+        <v>2015</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" t="s">
+        <v>199</v>
+      </c>
+      <c r="G6" t="s">
+        <v>196</v>
+      </c>
+      <c r="H6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7">
+        <v>2015</v>
+      </c>
+      <c r="D7" t="s">
+        <v>199</v>
+      </c>
+      <c r="E7" t="s">
+        <v>199</v>
+      </c>
+      <c r="G7" t="s">
+        <v>196</v>
+      </c>
+      <c r="H7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8">
+        <v>2015</v>
+      </c>
+      <c r="D8" t="s">
+        <v>199</v>
+      </c>
+      <c r="E8" t="s">
+        <v>199</v>
+      </c>
+      <c r="G8" t="s">
+        <v>196</v>
+      </c>
+      <c r="H8" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9">
+        <v>2014</v>
+      </c>
+      <c r="D9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10">
+        <v>2014</v>
+      </c>
+      <c r="D10" t="s">
+        <v>199</v>
+      </c>
+      <c r="E10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Revert "data entry, added ugliest search box of all time, unsuccessfuly tried to fix datatable"
This reverts commit 138638f9dea6a7884a2dcd70635d73e66004dd14.
</commit_message>
<xml_diff>
--- a/2.0/data/datatable.xlsx
+++ b/2.0/data/datatable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="2325" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="2325"/>
   </bookViews>
   <sheets>
     <sheet name="370 Projects" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="158">
   <si>
     <t>Title</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Semester</t>
+  </si>
+  <si>
+    <t>Source (URL or file location?)</t>
   </si>
   <si>
     <t>Treading Water: The Dutch Reliance on Water Management</t>
@@ -519,213 +522,6 @@
   </si>
   <si>
     <t>Jessica Shen</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Edinburgh Marathon Course Map</t>
-  </si>
-  <si>
-    <t>Jacqueline Heller</t>
-  </si>
-  <si>
-    <t>sports, elevation, race</t>
-  </si>
-  <si>
-    <t>The Alphorn-Man Triathlon of New Glarus</t>
-  </si>
-  <si>
-    <t>Jackson Gabriel</t>
-  </si>
-  <si>
-    <t>sports, race</t>
-  </si>
-  <si>
-    <t>Greg Lehner</t>
-  </si>
-  <si>
-    <t>How Many Big Macs Can You Buy?</t>
-  </si>
-  <si>
-    <t>economics, world map, gross domestic product</t>
-  </si>
-  <si>
-    <t>Mammal Diversity of North America</t>
-  </si>
-  <si>
-    <t>Grace Shellinger</t>
-  </si>
-  <si>
-    <t>The Frontline of the Battle Against Asian Carp in the Great Lakes Drainage Basin</t>
-  </si>
-  <si>
-    <t>Erin Hamilton</t>
-  </si>
-  <si>
-    <t>environment, invasive species</t>
-  </si>
-  <si>
-    <t>David Rhoten</t>
-  </si>
-  <si>
-    <t>Reconstructing Iraq, Summer 2003: 928 Engineer Group Survey and Design</t>
-  </si>
-  <si>
-    <t>Syria, Turkey, Iraq, Middle East</t>
-  </si>
-  <si>
-    <t>October 2011 Northern Hemisphere Jets and Superpositions</t>
-  </si>
-  <si>
-    <t>Croix Christenson</t>
-  </si>
-  <si>
-    <t>weather, meteorology, polar jet, subtropical jet, choropleth</t>
-  </si>
-  <si>
-    <t>Protecting the Penokee Range from Irresponsible Iron Mining</t>
-  </si>
-  <si>
-    <t>Christy Stamos</t>
-  </si>
-  <si>
-    <t>Wisconsin, Madison, Green Bay, Milwaukee, Wisconsin League of Conservation Voters</t>
-  </si>
-  <si>
-    <t>Casey Dahl</t>
-  </si>
-  <si>
-    <t>What Is Local? Dane County Farmers Market Vendor Locations in 2009</t>
-  </si>
-  <si>
-    <t>farmer's market, local food, health, Dane County Farmers' Market, choropleth</t>
-  </si>
-  <si>
-    <t>Blake Draper</t>
-  </si>
-  <si>
-    <t>Mapping a Watershed: Three Views of the Yahara Watershed for Public Outreach and Education</t>
-  </si>
-  <si>
-    <t>choropleth, dot density</t>
-  </si>
-  <si>
-    <t>America's Pastime? Wins, Ticket Price, and Attendance for Major League Baseball Franchises, 2011</t>
-  </si>
-  <si>
-    <t>Bryan Plaster</t>
-  </si>
-  <si>
-    <t>proportional symbol, choropleth, United States, spors</t>
-  </si>
-  <si>
-    <t>The Dirty Truth About Coal</t>
-  </si>
-  <si>
-    <t>Amanda Kannard</t>
-  </si>
-  <si>
-    <t>coal plants, Wisconsin, proportional symbol, bivariate choropleth, health, respiratory disease</t>
-  </si>
-  <si>
-    <t>Spain's Influence on the World</t>
-  </si>
-  <si>
-    <t>Ari Malman</t>
-  </si>
-  <si>
-    <t>language, world map, choropleth, history</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>Robinson AC and RE Roth</t>
-  </si>
-  <si>
-    <t>Buckingham TMA and RE Roth.</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Special Issue on Cognition, Representation, and Behavior sponsored by the International Cartography Association (ICA).</t>
-  </si>
-  <si>
-    <t>Second Special Digital Issue.</t>
-  </si>
-  <si>
-    <t>Cartographic Perspectives 66. [open access]</t>
-  </si>
-  <si>
-    <t>Cartographic Perspectives 77. [open access]</t>
-  </si>
-  <si>
-    <t>Wireframing for interactive &amp; web-based mapping: Designing the NOAA Lake Level Viewer. </t>
-  </si>
-  <si>
-    <t>Cartography and Geographic Information Science</t>
-  </si>
-  <si>
-    <t>Roth RE. </t>
-  </si>
-  <si>
-    <t>Roth RE, D Hart, R Mead, and C Quinn.</t>
-  </si>
-  <si>
-    <t>forthcoming</t>
-  </si>
-  <si>
-    <t>Cartographica. 50(2).</t>
-  </si>
-  <si>
-    <t>Interactivity and Cartography: A contemporary perspective on UI/UX design from geospatial professionals. </t>
-  </si>
-  <si>
-    <t>Tambopata transformed: Using web mapping to enhance a geography course exercise about forest conservation. </t>
-  </si>
-  <si>
-    <t>Weiss MJ, M Omri, G White, RE Roth, and LC Naughton-Treves. 2015.</t>
-  </si>
-  <si>
-    <t>The Journal of Maps. 11(3): 525-533. [uncorrected pre-print]</t>
-  </si>
-  <si>
-    <t>User-centered design for interactive maps: A case study in crime analysis. </t>
-  </si>
-  <si>
-    <t>Roth RE, KS Ross, and AM MacEachren.</t>
-  </si>
-  <si>
-    <t> International Journal of Geo-Information. 4(1): 262-301. [open access]</t>
-  </si>
-  <si>
-    <t>Roth RE, C Quinn, and D Hart. 2015.</t>
-  </si>
-  <si>
-    <t>The competitive analysis method for evaluating water level visualization tools.</t>
-  </si>
-  <si>
-    <t>In: A. Vondrakova, J. Brus, and V. Vozenilek (eds) Modern Trends in Cartography, Lecture Notes in Geoinformation and Cartography. Chapter 19: 241-256. [uncorrected pre-print]</t>
-  </si>
-  <si>
-    <t>Roth RE, RG Donohue, CM Sack, T Wallace, and T Buckingham.</t>
-  </si>
-  <si>
-    <t>Keeping pace with evolving open source web mapping technologies.</t>
-  </si>
-  <si>
-    <t>Dong W, H Liao, RE Roth, and S Wang.</t>
-  </si>
-  <si>
-    <t>Cartographic Perspectives. 78: 25-52. [open access]</t>
-  </si>
-  <si>
-    <t>Eye tracking to explore the potential of enhanced imagery basemaps in web mapping.</t>
-  </si>
-  <si>
-    <t>The Cartographic Journal. 51(4): 313-329. [uncorrected pre-print]</t>
   </si>
 </sst>
 </file>
@@ -862,23 +658,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -914,23 +693,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1083,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1097,12 +859,12 @@
     <col min="10" max="10" width="24.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1114,1634 +876,1377 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>2012</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
       <c r="C3">
         <v>2012</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>2012</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>2012</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2012</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
       <c r="C7">
         <v>2012</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
       <c r="C8">
         <v>2012</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>2012</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
       <c r="C10">
         <v>2012</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
       <c r="C11">
         <v>2012</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12">
         <v>2012</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13">
         <v>2012</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>2012</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15">
         <v>2012</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
       <c r="C16">
         <v>2012</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17">
         <v>2012</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
       <c r="C18">
         <v>2012</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
       <c r="C19">
         <v>2012</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>2012</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21">
         <v>2012</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22">
         <v>2012</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
       <c r="C24">
         <v>2012</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
       <c r="C25">
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26">
         <v>2012</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>2012</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28">
         <v>2012</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
         <v>61</v>
       </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
       <c r="C29">
         <v>2012</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C30">
         <v>2012</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31">
         <v>2012</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C32">
         <v>2012</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
         <v>70</v>
       </c>
-      <c r="B33" t="s">
-        <v>69</v>
-      </c>
       <c r="C33">
         <v>2012</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C34">
         <v>2012</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" t="s">
         <v>74</v>
       </c>
-      <c r="B35" t="s">
-        <v>73</v>
-      </c>
       <c r="C35">
         <v>2012</v>
       </c>
       <c r="D35" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>2012</v>
       </c>
       <c r="D36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C37">
         <v>2012</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" t="s">
         <v>80</v>
       </c>
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
       <c r="C38">
         <v>2012</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <v>2012</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>2012</v>
       </c>
       <c r="D40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C41">
         <v>2012</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G41" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C42">
         <v>2012</v>
       </c>
       <c r="D42" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G42" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C43">
         <v>2012</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G43" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
         <v>92</v>
       </c>
-      <c r="B44" t="s">
-        <v>91</v>
-      </c>
       <c r="C44">
         <v>2012</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G44" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G45" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" t="s">
         <v>96</v>
       </c>
-      <c r="B46" t="s">
-        <v>95</v>
-      </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G47" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C48">
         <v>2012</v>
       </c>
       <c r="D48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G48" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
         <v>102</v>
       </c>
-      <c r="B49" t="s">
-        <v>101</v>
-      </c>
       <c r="C49">
         <v>2012</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" t="s">
         <v>104</v>
       </c>
-      <c r="B50" t="s">
-        <v>103</v>
-      </c>
       <c r="C50">
         <v>2012</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C51">
         <v>2012</v>
       </c>
       <c r="D51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E51" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
         <v>108</v>
       </c>
-      <c r="B52" t="s">
-        <v>107</v>
-      </c>
       <c r="C52">
         <v>2012</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G52" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
         <v>110</v>
       </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
       <c r="C53">
         <v>2012</v>
       </c>
       <c r="D53" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G53" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
         <v>112</v>
       </c>
-      <c r="B54" t="s">
-        <v>111</v>
-      </c>
       <c r="C54">
         <v>2012</v>
       </c>
       <c r="D54" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E54" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G54" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C55">
         <v>2011</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E55" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G55" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
+        <v>121</v>
+      </c>
+      <c r="B56" t="s">
         <v>120</v>
-      </c>
-      <c r="B56" t="s">
-        <v>119</v>
       </c>
       <c r="C56">
         <v>2011</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F56" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G56" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C57">
         <v>2011</v>
       </c>
       <c r="D57" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E57" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G57" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B58" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C58">
         <v>2011</v>
       </c>
       <c r="D58" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F58" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G58" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" t="s">
         <v>129</v>
-      </c>
-      <c r="B59" t="s">
-        <v>128</v>
       </c>
       <c r="C59">
         <v>2011</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G59" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C60">
         <v>2011</v>
       </c>
       <c r="D60" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F60" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G60" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B61" t="s">
         <v>135</v>
-      </c>
-      <c r="B61" t="s">
-        <v>134</v>
       </c>
       <c r="C61">
         <v>2011</v>
       </c>
       <c r="D61" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E61" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F61" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G61" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B62" t="s">
         <v>138</v>
-      </c>
-      <c r="B62" t="s">
-        <v>137</v>
       </c>
       <c r="C62">
         <v>2011</v>
       </c>
       <c r="D62" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E62" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F62" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G62" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B63" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C63">
         <v>2011</v>
       </c>
       <c r="D63" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F63" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G63" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C64">
         <v>2011</v>
       </c>
       <c r="D64" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E64" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F64" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B65" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C65">
         <v>2011</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E65" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F65" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>151</v>
+      </c>
+      <c r="B66" t="s">
         <v>150</v>
-      </c>
-      <c r="B66" t="s">
-        <v>149</v>
       </c>
       <c r="C66">
         <v>2011</v>
       </c>
       <c r="D66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E66" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F66" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" t="s">
         <v>153</v>
-      </c>
-      <c r="B67" t="s">
-        <v>152</v>
       </c>
       <c r="C67">
         <v>2011</v>
       </c>
       <c r="D67" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F67" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B68" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C68">
         <v>2011</v>
       </c>
       <c r="D68" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E68" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>158</v>
-      </c>
-      <c r="B69" t="s">
-        <v>159</v>
-      </c>
-      <c r="C69">
-        <v>2011</v>
-      </c>
-      <c r="D69" t="s">
-        <v>67</v>
-      </c>
-      <c r="E69" t="s">
-        <v>7</v>
-      </c>
-      <c r="F69" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>161</v>
-      </c>
-      <c r="B70" t="s">
-        <v>162</v>
-      </c>
-      <c r="C70">
-        <v>2011</v>
-      </c>
-      <c r="D70" t="s">
-        <v>67</v>
-      </c>
-      <c r="E70" t="s">
-        <v>7</v>
-      </c>
-      <c r="F70" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>165</v>
-      </c>
-      <c r="B71" t="s">
-        <v>164</v>
-      </c>
-      <c r="C71">
-        <v>2011</v>
-      </c>
-      <c r="D71" t="s">
-        <v>67</v>
-      </c>
-      <c r="E71" t="s">
-        <v>7</v>
-      </c>
-      <c r="F71" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>167</v>
-      </c>
-      <c r="B72" t="s">
-        <v>168</v>
-      </c>
-      <c r="C72">
-        <v>2011</v>
-      </c>
-      <c r="D72" t="s">
-        <v>67</v>
-      </c>
-      <c r="E72" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>169</v>
-      </c>
-      <c r="B73" t="s">
-        <v>170</v>
-      </c>
-      <c r="C73">
-        <v>2011</v>
-      </c>
-      <c r="D73" t="s">
-        <v>67</v>
-      </c>
-      <c r="E73" t="s">
-        <v>7</v>
-      </c>
-      <c r="F73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>173</v>
-      </c>
-      <c r="B74" t="s">
-        <v>172</v>
-      </c>
-      <c r="C74">
-        <v>2011</v>
-      </c>
-      <c r="D74" t="s">
-        <v>67</v>
-      </c>
-      <c r="E74" t="s">
-        <v>7</v>
-      </c>
-      <c r="F74" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>175</v>
-      </c>
-      <c r="B75" t="s">
-        <v>176</v>
-      </c>
-      <c r="C75">
-        <v>2011</v>
-      </c>
-      <c r="D75" t="s">
-        <v>67</v>
-      </c>
-      <c r="E75" t="s">
-        <v>7</v>
-      </c>
-      <c r="F75" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>178</v>
-      </c>
-      <c r="B76" t="s">
-        <v>179</v>
-      </c>
-      <c r="C76">
-        <v>2011</v>
-      </c>
-      <c r="D76" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>182</v>
-      </c>
-      <c r="B77" t="s">
-        <v>181</v>
-      </c>
-      <c r="C77">
-        <v>2011</v>
-      </c>
-      <c r="D77" t="s">
-        <v>67</v>
-      </c>
-      <c r="E77" t="s">
-        <v>7</v>
-      </c>
-      <c r="F77" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>185</v>
-      </c>
-      <c r="B78" t="s">
-        <v>184</v>
-      </c>
-      <c r="C78">
-        <v>2011</v>
-      </c>
-      <c r="D78" t="s">
-        <v>67</v>
-      </c>
-      <c r="E78" t="s">
-        <v>7</v>
-      </c>
-      <c r="F78" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>187</v>
-      </c>
-      <c r="B79" t="s">
-        <v>188</v>
-      </c>
-      <c r="C79">
-        <v>2011</v>
-      </c>
-      <c r="D79" t="s">
-        <v>67</v>
-      </c>
-      <c r="E79" t="s">
-        <v>7</v>
-      </c>
-      <c r="F79" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>190</v>
-      </c>
-      <c r="B80" t="s">
-        <v>191</v>
-      </c>
-      <c r="C80">
-        <v>2011</v>
-      </c>
-      <c r="D80" t="s">
-        <v>67</v>
-      </c>
-      <c r="E80" t="s">
-        <v>7</v>
-      </c>
-      <c r="F80" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>193</v>
-      </c>
-      <c r="B81" t="s">
-        <v>194</v>
-      </c>
-      <c r="C81">
-        <v>2011</v>
-      </c>
-      <c r="D81" t="s">
-        <v>67</v>
-      </c>
-      <c r="E81" t="s">
-        <v>7</v>
-      </c>
-      <c r="F81" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2755,310 +2260,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2">
-        <v>2014</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3">
-        <v>2010</v>
-      </c>
-      <c r="D3" t="s">
-        <v>199</v>
-      </c>
-      <c r="E3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G3" t="s">
-        <v>196</v>
-      </c>
-      <c r="H3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>204</v>
-      </c>
-      <c r="B4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C4">
-        <v>2014</v>
-      </c>
-      <c r="D4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E4" t="s">
-        <v>199</v>
-      </c>
-      <c r="G4" t="s">
-        <v>196</v>
-      </c>
-      <c r="H4" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D5" t="s">
-        <v>199</v>
-      </c>
-      <c r="E5" t="s">
-        <v>199</v>
-      </c>
-      <c r="G5" t="s">
-        <v>196</v>
-      </c>
-      <c r="H5" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" t="s">
-        <v>212</v>
-      </c>
-      <c r="C6">
-        <v>2015</v>
-      </c>
-      <c r="D6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E6" t="s">
-        <v>199</v>
-      </c>
-      <c r="G6" t="s">
-        <v>196</v>
-      </c>
-      <c r="H6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>214</v>
-      </c>
-      <c r="B7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7">
-        <v>2015</v>
-      </c>
-      <c r="D7" t="s">
-        <v>199</v>
-      </c>
-      <c r="E7" t="s">
-        <v>199</v>
-      </c>
-      <c r="G7" t="s">
-        <v>196</v>
-      </c>
-      <c r="H7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>218</v>
-      </c>
-      <c r="B8" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8">
-        <v>2015</v>
-      </c>
-      <c r="D8" t="s">
-        <v>199</v>
-      </c>
-      <c r="E8" t="s">
-        <v>199</v>
-      </c>
-      <c r="G8" t="s">
-        <v>196</v>
-      </c>
-      <c r="H8" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B9" t="s">
-        <v>220</v>
-      </c>
-      <c r="C9">
-        <v>2014</v>
-      </c>
-      <c r="D9" t="s">
-        <v>199</v>
-      </c>
-      <c r="E9" t="s">
-        <v>199</v>
-      </c>
-      <c r="G9" t="s">
-        <v>196</v>
-      </c>
-      <c r="H9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>224</v>
-      </c>
-      <c r="B10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C10">
-        <v>2014</v>
-      </c>
-      <c r="D10" t="s">
-        <v>199</v>
-      </c>
-      <c r="E10" t="s">
-        <v>199</v>
-      </c>
-      <c r="G10" t="s">
-        <v>196</v>
-      </c>
-      <c r="H10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G11" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G12" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G13" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G14" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="G16" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G19" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G21" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.45">
-      <c r="G22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>